<commit_message>
Fixes made to theta and hydrogen (G.Inga removed from 8 and 9 gt runs)
</commit_message>
<xml_diff>
--- a/SATIM/RES Diagrams/RES_detailed_v01.xlsx
+++ b/SATIM/RES Diagrams/RES_detailed_v01.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE\SATIM\RES Diagrams\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B20901C-A9D1-4E1C-B7B7-64B2A202C536}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A2C2538-44DE-4749-8F1B-4CA6CCE8CE22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3180" yWindow="-17385" windowWidth="26475" windowHeight="15570" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1170" windowWidth="28800" windowHeight="14745" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SATIMFullRESNewCoal" sheetId="7" r:id="rId1"/>
     <sheet name="SATIM-EL" sheetId="6" r:id="rId2"/>
-    <sheet name="SATIMFullRES" sheetId="1" r:id="rId3"/>
-    <sheet name="SATIMTPPR" sheetId="5" r:id="rId4"/>
-    <sheet name="eSAGE_oldLink" sheetId="2" r:id="rId5"/>
-    <sheet name="eSAGE_NewLink" sheetId="4" r:id="rId6"/>
+    <sheet name="SATIMFullRES_wPics" sheetId="8" r:id="rId3"/>
+    <sheet name="SATIMFullRES" sheetId="1" r:id="rId4"/>
+    <sheet name="SATIMTPPR" sheetId="5" r:id="rId5"/>
+    <sheet name="eSAGE_oldLink" sheetId="2" r:id="rId6"/>
+    <sheet name="eSAGE_NewLink" sheetId="4" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="60">
   <si>
     <t>Coal Mines</t>
   </si>
@@ -510,7 +511,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -612,6 +613,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -627,6 +649,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>42333</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>147108</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{485EA479-3673-4B9B-8545-8050E72815C5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3884083" y="2730500"/>
+          <a:ext cx="590550" cy="295275"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1485,7 +1556,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB56E853-3E2D-4572-B8A0-39136E124886}">
   <dimension ref="A1:T42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="C1" sqref="C1:P24"/>
     </sheetView>
   </sheetViews>
@@ -1860,6 +1931,500 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C44A2E2C-2D45-4595-92FF-BFA9BB717826}">
+  <dimension ref="A1:U42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="9.140625" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" customWidth="1"/>
+    <col min="4" max="4" width="3.85546875" customWidth="1"/>
+    <col min="5" max="6" width="3.5703125" customWidth="1"/>
+    <col min="7" max="8" width="4" customWidth="1"/>
+    <col min="9" max="9" width="23.140625" customWidth="1"/>
+    <col min="10" max="11" width="3.5703125" customWidth="1"/>
+    <col min="12" max="12" width="3.85546875" customWidth="1"/>
+    <col min="13" max="13" width="22.5703125" customWidth="1"/>
+    <col min="14" max="17" width="3.5703125" customWidth="1"/>
+    <col min="18" max="18" width="3.85546875" customWidth="1"/>
+    <col min="19" max="19" width="22.5703125" customWidth="1"/>
+    <col min="20" max="21" width="3.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" ht="91.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="42" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="H1" s="2"/>
+      <c r="I1" s="42" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="M1" s="42" t="s">
+        <v>33</v>
+      </c>
+      <c r="N1" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="O1" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="P1" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="S1" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="T1" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="U1" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="E2" s="5"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="N2" s="4"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="T2" s="5"/>
+      <c r="U2" s="5"/>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="42"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
+      <c r="Q3" s="5"/>
+      <c r="T3" s="5"/>
+      <c r="U3" s="5"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="D4" s="42"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="44" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="M4" s="42"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="15"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="6"/>
+      <c r="S4" s="42"/>
+      <c r="T4" s="5"/>
+      <c r="U4" s="5"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="C5" s="42"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="42"/>
+      <c r="I5" s="45"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="8"/>
+      <c r="Q5" s="8"/>
+      <c r="R5" s="13"/>
+      <c r="S5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="T5" s="4"/>
+      <c r="U5" s="5"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="C6" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="7"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="I6" s="46"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="N6" s="4"/>
+      <c r="O6" s="18"/>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="32"/>
+      <c r="S6" s="4"/>
+      <c r="T6" s="5"/>
+      <c r="U6" s="5"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="C7" s="4"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="44" t="s">
+        <v>36</v>
+      </c>
+      <c r="J7" s="8"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="32"/>
+      <c r="M7" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="N7" s="5"/>
+      <c r="O7" s="11"/>
+      <c r="P7" s="11"/>
+      <c r="Q7" s="5"/>
+      <c r="R7" s="12"/>
+      <c r="T7" s="5"/>
+      <c r="U7" s="5"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="C8" s="42"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="42"/>
+      <c r="I8" s="45"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="12"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="4"/>
+      <c r="R8" s="13"/>
+      <c r="S8" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="T8" s="4"/>
+      <c r="U8" s="5"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="C9" s="42"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="15"/>
+      <c r="I9" s="46"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="11"/>
+      <c r="R9" s="32"/>
+      <c r="S9" s="4"/>
+      <c r="T9" s="5"/>
+      <c r="U9" s="5"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="C10" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="7"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="44" t="s">
+        <v>31</v>
+      </c>
+      <c r="J10" s="8"/>
+      <c r="K10" s="4"/>
+      <c r="O10" s="11"/>
+      <c r="P10" s="11"/>
+      <c r="Q10" s="11"/>
+      <c r="T10" s="5"/>
+      <c r="U10" s="5"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="C11" s="4"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="42"/>
+      <c r="I11" s="45"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="11"/>
+      <c r="O11" s="11"/>
+      <c r="P11" s="11"/>
+      <c r="Q11" s="11"/>
+      <c r="T11" s="5"/>
+      <c r="U11" s="5"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="C12" s="42"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="36"/>
+      <c r="I12" s="47"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="O12" s="11"/>
+      <c r="P12" s="11"/>
+      <c r="Q12" s="5"/>
+      <c r="S12" s="42"/>
+      <c r="T12" s="5"/>
+      <c r="U12" s="5"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="C13" s="42"/>
+      <c r="D13" s="42"/>
+      <c r="E13" s="5"/>
+      <c r="G13" s="15"/>
+      <c r="I13" s="46"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="O13" s="11"/>
+      <c r="P13" s="11"/>
+      <c r="Q13" s="11"/>
+      <c r="T13" s="5"/>
+      <c r="U13" s="5"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A14" s="12"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="5"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="J14" s="8"/>
+      <c r="K14" s="11"/>
+      <c r="O14" s="11"/>
+      <c r="P14" s="4"/>
+      <c r="Q14" s="8"/>
+      <c r="R14" s="13"/>
+      <c r="S14" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="T14" s="4"/>
+      <c r="U14" s="4"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="C15" s="42"/>
+      <c r="D15" s="42"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="42"/>
+      <c r="I15" s="45"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="11"/>
+      <c r="O15" s="11"/>
+      <c r="P15" s="11"/>
+      <c r="Q15" s="3"/>
+      <c r="R15" s="32"/>
+      <c r="S15" s="4"/>
+      <c r="T15" s="5"/>
+      <c r="U15" s="5"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="48"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="13"/>
+      <c r="M16" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="N16" s="7"/>
+      <c r="O16" s="4"/>
+      <c r="P16" s="8"/>
+      <c r="Q16" s="5"/>
+      <c r="S16" s="42"/>
+      <c r="T16" s="5"/>
+      <c r="U16" s="5"/>
+    </row>
+    <row r="17" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C17" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" s="7"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="46"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="14"/>
+      <c r="O17" s="11"/>
+      <c r="P17" s="3"/>
+      <c r="Q17" s="11"/>
+      <c r="S17" s="42"/>
+      <c r="T17" s="5"/>
+      <c r="U17" s="5"/>
+    </row>
+    <row r="18" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C18" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" s="42"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="44" t="s">
+        <v>45</v>
+      </c>
+      <c r="J18" s="8"/>
+      <c r="K18" s="11"/>
+      <c r="O18" s="11"/>
+      <c r="P18" s="11"/>
+      <c r="Q18" s="11"/>
+      <c r="R18" s="13"/>
+      <c r="S18" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="T18" s="4"/>
+      <c r="U18" s="4"/>
+    </row>
+    <row r="19" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="F19" s="30"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="49"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="13"/>
+      <c r="M19" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="N19" s="7"/>
+      <c r="O19" s="4"/>
+      <c r="P19" s="8"/>
+      <c r="Q19" s="8"/>
+      <c r="S19" s="4"/>
+      <c r="T19" s="5"/>
+      <c r="U19" s="5"/>
+    </row>
+    <row r="20" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C20" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" s="7"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="I20" s="45"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="32"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="14"/>
+      <c r="O20" s="11"/>
+      <c r="P20" s="5"/>
+      <c r="Q20" s="5"/>
+      <c r="S20" s="42"/>
+      <c r="T20" s="5"/>
+      <c r="U20" s="5"/>
+    </row>
+    <row r="21" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C21" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" s="42"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="M21" s="42"/>
+      <c r="N21" s="14"/>
+      <c r="O21" s="11"/>
+      <c r="P21" s="5"/>
+      <c r="Q21" s="5"/>
+      <c r="T21" s="5"/>
+      <c r="U21" s="5"/>
+    </row>
+    <row r="22" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="E22" s="5"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="N22" s="14"/>
+      <c r="O22" s="11"/>
+      <c r="P22" s="5"/>
+      <c r="Q22" s="5"/>
+      <c r="T22" s="5"/>
+      <c r="U22" s="5"/>
+    </row>
+    <row r="24" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="J24" s="12"/>
+    </row>
+    <row r="42" spans="13:19" x14ac:dyDescent="0.25">
+      <c r="M42" s="12"/>
+      <c r="S42" s="12"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U42"/>
   <sheetViews>
@@ -2348,7 +2913,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9158AE5F-26FB-4763-90C8-4E5345128817}">
   <dimension ref="C1:J41"/>
   <sheetViews>
@@ -2529,7 +3094,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="C1:Y39"/>
   <sheetViews>
@@ -2552,25 +3117,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="3:25" x14ac:dyDescent="0.25">
-      <c r="E1" s="42" t="s">
+      <c r="E1" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
       <c r="K1" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="M1" s="42" t="s">
+      <c r="M1" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="N1" s="42"/>
-      <c r="O1" s="42"/>
-      <c r="P1" s="42"/>
-      <c r="Q1" s="42"/>
-      <c r="R1" s="42"/>
-      <c r="S1" s="42"/>
+      <c r="N1" s="43"/>
+      <c r="O1" s="43"/>
+      <c r="P1" s="43"/>
+      <c r="Q1" s="43"/>
+      <c r="R1" s="43"/>
+      <c r="S1" s="43"/>
       <c r="U1" s="14" t="s">
         <v>15</v>
       </c>
@@ -3414,7 +3979,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A1C4BB2-A0B5-4FE6-912B-169A6B7F726F}">
   <dimension ref="C1:AA39"/>
   <sheetViews>
@@ -3437,30 +4002,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="3:27" x14ac:dyDescent="0.25">
-      <c r="D1" s="42" t="s">
+      <c r="D1" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
-      <c r="K1" s="42"/>
-      <c r="L1" s="42"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
+      <c r="L1" s="43"/>
       <c r="M1" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="O1" s="42" t="s">
+      <c r="O1" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="P1" s="42"/>
-      <c r="Q1" s="42"/>
-      <c r="R1" s="42"/>
-      <c r="S1" s="42"/>
-      <c r="T1" s="42"/>
-      <c r="U1" s="42"/>
-      <c r="V1" s="42"/>
+      <c r="P1" s="43"/>
+      <c r="Q1" s="43"/>
+      <c r="R1" s="43"/>
+      <c r="S1" s="43"/>
+      <c r="T1" s="43"/>
+      <c r="U1" s="43"/>
+      <c r="V1" s="43"/>
       <c r="W1" s="14" t="s">
         <v>15</v>
       </c>

</xml_diff>